<commit_message>
LiRI feedback - change RQ1 table
</commit_message>
<xml_diff>
--- a/01_data/Leap_Q_combined.xlsx
+++ b/01_data/Leap_Q_combined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nataliehennig/Documents/language-and-emotion/01_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D58CDB9-AD14-A14F-985E-E3B69D9280BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B2BA5D-283B-DE47-9647-5F4848D15F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{5D63B9C6-4C47-024D-A9E8-5A261856B1C4}"/>
   </bookViews>
@@ -3027,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0837D9BE-5256-AA4D-822C-71D8DD948064}">
   <dimension ref="A1:N539"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" zoomScale="137" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A523" zoomScale="137" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5675,7 +5675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -6108,8 +6108,11 @@
       <c r="M75">
         <v>20</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -6150,7 +6153,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -6191,7 +6194,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -6232,7 +6235,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -6273,7 +6276,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -6314,7 +6317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -6355,7 +6358,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -6396,7 +6399,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -6437,7 +6440,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -6478,7 +6481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -6519,7 +6522,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>85</v>
       </c>
@@ -6560,7 +6563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -6601,7 +6604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>87</v>
       </c>
@@ -6642,7 +6645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -6683,7 +6686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>89</v>
       </c>
@@ -6724,7 +6727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -6765,7 +6768,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>91</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -6847,7 +6850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>93</v>
       </c>
@@ -6870,8 +6873,11 @@
       <c r="M94">
         <v>20</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -6912,7 +6918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>95</v>
       </c>

</xml_diff>